<commit_message>
Migliorato filtro in UI
</commit_message>
<xml_diff>
--- a/Materiale da GD/Appunti su colonne.xlsx
+++ b/Materiale da GD/Appunti su colonne.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18915" windowHeight="10740" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18915" windowHeight="10740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping campi" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="Grafici per le slides" sheetId="2" r:id="rId3"/>
+    <sheet name="Grafici per le slides" sheetId="2" r:id="rId2"/>
+    <sheet name="Suddivisione boxes in the slide" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -3034,6 +3034,137 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26:J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3370,135 +3501,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26:J27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>182</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>